<commit_message>
update Kostenplan again + pdf
</commit_message>
<xml_diff>
--- a/Kostenplan.xlsx
+++ b/Kostenplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Russen-Versenken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C414376-A9D1-48C3-94CB-1085C59EE738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD009ACD-96B9-4908-B923-8813434A4ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{B78EB2A0-5797-4C8A-B57A-20925B587D29}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Projektkostenarten</t>
   </si>
@@ -101,9 +101,6 @@
     <t>320€/Monat/User, ca. 2€/Std. , 2User</t>
   </si>
   <si>
-    <t xml:space="preserve"> 100€/Std., ca. 10 Arbeitsstunden</t>
-  </si>
-  <si>
     <t>80€/Std./Mitarbeiter, 2 Mitarbeiter je 75 Std.</t>
   </si>
   <si>
@@ -117,6 +114,15 @@
   </si>
   <si>
     <t>130€/Std., ca  10 Arbeitsstunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 100€/Std., ca. 8 Arbeitsstunden</t>
+  </si>
+  <si>
+    <t>Projekt:</t>
+  </si>
+  <si>
+    <t>Russen Versenken</t>
   </si>
 </sst>
 </file>
@@ -696,7 +702,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0A9F9C-797E-4F0B-A650-73FA7D7A53D4}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
@@ -709,8 +715,16 @@
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="2:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -724,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
@@ -732,7 +746,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -744,12 +758,12 @@
       </c>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="15">
         <f>250*2*3/4</f>
@@ -757,7 +771,7 @@
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
@@ -768,7 +782,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
@@ -776,7 +790,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -788,7 +802,7 @@
       </c>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -801,12 +815,12 @@
       </c>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="15">
         <f>130*10</f>
@@ -814,32 +828,32 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D12" s="15">
-        <f>100*10</f>
-        <v>1000</v>
+        <f>100*8</f>
+        <v>800</v>
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D13" s="15">
         <v>900</v>
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="12" t="s">
         <v>12</v>
       </c>
@@ -847,10 +861,10 @@
       <c r="D14" s="16"/>
       <c r="E14" s="20">
         <f>SUM(D9:D13)</f>
-        <v>3510.5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>3310.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="10" t="s">
         <v>13</v>
       </c>
@@ -858,12 +872,12 @@
       <c r="D15" s="17"/>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="15">
         <f>80*75*2</f>
@@ -890,12 +904,12 @@
       <c r="D18" s="18"/>
       <c r="E18" s="22">
         <f>SUM(E7,E14,E17)</f>
-        <v>15975.5</v>
+        <v>15775.5</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>